<commit_message>
Updated logic for 'Import Users from Excel'
</commit_message>
<xml_diff>
--- a/public/excel/test_excel_users.xlsx
+++ b/public/excel/test_excel_users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoni\Documnets\Deltion\extraOpd\laravel\projectkaarten\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43934997-6290-4AD1-B810-02371497FC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C765829C-BB29-4F65-AFC7-DB9014852059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" xr2:uid="{03F5CB61-3604-4CB3-BA31-7ED94BDCDEC5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>full_name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Excel1</t>
   </si>
   <si>
-    <t>excel1</t>
-  </si>
-  <si>
     <t>excel1@test</t>
   </si>
   <si>
@@ -68,16 +65,22 @@
     <t>excel4@test</t>
   </si>
   <si>
-    <t>excel3</t>
-  </si>
-  <si>
-    <t>excel4</t>
-  </si>
-  <si>
     <t>Excel3</t>
   </si>
   <si>
     <t>Excel4</t>
+  </si>
+  <si>
+    <t>excel11</t>
+  </si>
+  <si>
+    <t>excel12</t>
+  </si>
+  <si>
+    <t>excel33</t>
+  </si>
+  <si>
+    <t>excel44</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,10 +490,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>5</v>
@@ -501,10 +504,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -512,13 +515,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -526,13 +529,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Updated 'Excel users import' system. Set Dutch as the default language for validation messages.
</commit_message>
<xml_diff>
--- a/public/excel/test_excel_users.xlsx
+++ b/public/excel/test_excel_users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoni\Documnets\Deltion\extraOpd\laravel\projectkaarten\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43934997-6290-4AD1-B810-02371497FC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7DBC09-1DE9-4F3F-BADE-B33654644692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" xr2:uid="{03F5CB61-3604-4CB3-BA31-7ED94BDCDEC5}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{03F5CB61-3604-4CB3-BA31-7ED94BDCDEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>full_name</t>
   </si>
@@ -44,40 +44,16 @@
     <t>identifier</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>role_id</t>
+    <t>&lt;- Al in gebruik</t>
   </si>
   <si>
     <t>Excel1</t>
   </si>
   <si>
-    <t>excel1</t>
-  </si>
-  <si>
-    <t>excel1@test</t>
-  </si>
-  <si>
-    <t>excel2@test</t>
-  </si>
-  <si>
-    <t>excel3@test</t>
-  </si>
-  <si>
-    <t>excel4@test</t>
-  </si>
-  <si>
-    <t>excel3</t>
-  </si>
-  <si>
-    <t>excel4</t>
+    <t>Excel2</t>
   </si>
   <si>
     <t>Excel3</t>
-  </si>
-  <si>
-    <t>Excel4</t>
   </si>
 </sst>
 </file>
@@ -460,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C176F887-7C0B-4DE3-A027-C355FFA7B544}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,76 +451,37 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>971103</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
+      <c r="B3">
+        <v>971104</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>971102</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{BA9D3393-6E7F-4108-AC95-7BDDF9634B22}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{4E6DE612-F6FF-4E2E-AEAA-F25DDC85DDCF}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{23788EF5-A7AA-465C-90D9-661D7CF6441F}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{C51BDD32-FDAB-4A55-A006-86C6771F428A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>